<commit_message>
some of the codes has been changed here.
</commit_message>
<xml_diff>
--- a/PattRecClasses-bays-V3/PattRecClasses/PhaseEstimation/DataGenerator-ReaderTools/SyntheticAdaptive/HMMdataGenerator/DefaultEmissionProbs.xlsx
+++ b/PattRecClasses-bays-V3/PattRecClasses/PhaseEstimation/DataGenerator-ReaderTools/SyntheticAdaptive/HMMdataGenerator/DefaultEmissionProbs.xlsx
@@ -13,6 +13,10 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -352,313 +356,313 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D1">
-        <v>29.7</v>
+        <v>0.442943416743802</v>
       </c>
       <c r="E1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F1">
-        <v>10</v>
+        <v>6.8008934099110505E-2</v>
       </c>
       <c r="G1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J1">
-        <v>29.7</v>
+        <v>0.40641146779420501</v>
       </c>
       <c r="K1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L1">
-        <v>10</v>
+        <v>8.26361813628822E-2</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>29.7</v>
+        <v>0.52667637912673504</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>2.93348611438717E-2</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>29.7</v>
+        <v>0.40014397938859902</v>
       </c>
       <c r="H2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>10</v>
+        <v>4.3844780340794802E-2</v>
       </c>
       <c r="J2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>44.5</v>
+        <v>0.40989169877151099</v>
       </c>
       <c r="G3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>44.5</v>
+        <v>0.59010830122848901</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>44.5</v>
+        <v>0.34477421302384897</v>
       </c>
       <c r="D4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>44.5</v>
+        <v>0.65522578697615097</v>
       </c>
       <c r="J4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>49.1</v>
+        <v>0.656774168989399</v>
       </c>
       <c r="K5">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>25</v>
+        <v>0.343225831010601</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>49.1</v>
+        <v>0.80745471387803402</v>
       </c>
       <c r="E6">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>0.192545286121966</v>
       </c>
       <c r="G6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>49.1</v>
+        <v>0.72641020391599898</v>
       </c>
       <c r="H7">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>25</v>
+        <v>0.27358979608400102</v>
       </c>
       <c r="J7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>49.1</v>
+        <v>0.76759020332927297</v>
       </c>
       <c r="B8">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>25</v>
+        <v>0.232409796670727</v>
       </c>
       <c r="D8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>